<commit_message>
subiendo datos de alumnos
</commit_message>
<xml_diff>
--- a/extras/datos/captura datos Ing Sistemas FRANCISCO.xlsx
+++ b/extras/datos/captura datos Ing Sistemas FRANCISCO.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\boostrap studio\Servicio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\tutorias\extras\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A27DE50-8960-4DDF-89CA-1EC27A331123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C00A20-3165-46B0-8CE7-FD50924800E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{23017515-5504-4510-AD65-535B5F72485F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{23017515-5504-4510-AD65-535B5F72485F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="210">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -529,6 +530,138 @@
   </si>
   <si>
     <t>Abraham</t>
+  </si>
+  <si>
+    <t>FECHA DE NACIMIENTO</t>
+  </si>
+  <si>
+    <t>SEXO</t>
+  </si>
+  <si>
+    <t>CORREO ELECTRONICO</t>
+  </si>
+  <si>
+    <t>NUMERO DE TELEFONO</t>
+  </si>
+  <si>
+    <t>DIRECCION</t>
+  </si>
+  <si>
+    <t>CIUDAD</t>
+  </si>
+  <si>
+    <t>FOTO</t>
+  </si>
+  <si>
+    <t>direccion prueba</t>
+  </si>
+  <si>
+    <t>Juchitán</t>
+  </si>
+  <si>
+    <t>Tehuantepec</t>
+  </si>
+  <si>
+    <t>Ixtepec</t>
+  </si>
+  <si>
+    <t>Espinal</t>
+  </si>
+  <si>
+    <t>Unión Hidalgo</t>
+  </si>
+  <si>
+    <t>Chicapa</t>
+  </si>
+  <si>
+    <t>Ixtaltepec</t>
+  </si>
+  <si>
+    <t>Salina Cruz</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>/directory/img-person/RoelMorales.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/KarinaNuñez.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/KeniaOrozco.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/FátimaAntinio.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/VicenteAquino.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/BaudelAranjo.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/BrianBenefield.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/ClarissaZavala.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/LuisFuentes.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/MaytorRevuelta.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JorgeRobles.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/SergioRodas.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/GiovanniAlexanderMorales.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/DennisSabasOrozco.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/CarlosRobertoOrtiz.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/IsisYamileAltamirano.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/ItzuryAlejandraAquino.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/YosmarManuelAvedaño.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/KevinGabrielZarate.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JesusAntonioZarate.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/AlbaBeatrizAguilar.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/BrisaDonajiRuiz.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JairMichaelRuiz.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JoséGuillermoGonzales.jpg</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>/directory/img-person/UsmarIsaccMiguel.jpg</t>
   </si>
 </sst>
 </file>
@@ -603,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -618,6 +751,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F646EE8-7CC3-4945-A430-704E50C10C5B}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D61" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2324,4 +2462,1019 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2B5FE0-EEC0-4F6B-975E-DE53E3E1823C}">
+  <dimension ref="A1:S26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+    <col min="9" max="9" width="25.21875" customWidth="1"/>
+    <col min="10" max="10" width="51.88671875" customWidth="1"/>
+    <col min="12" max="12" width="198.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7">
+        <v>36449</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" t="str">
+        <f>CONCATENATE(B2,A2,LEFT(C2,2),"@gmail.com")</f>
+        <v>LopezMiguelUs@gmail.com</v>
+      </c>
+      <c r="G2" t="str">
+        <f ca="1">CONCATENATE("971",RANDBETWEEN(1111111,9999999))</f>
+        <v>9718643085</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J2" t="s">
+        <v>209</v>
+      </c>
+      <c r="L2" t="str">
+        <f ca="1">CONCATENATE("INSERT INTO 'persona' VALUES (",$S$2,C2,$S$2,",",$S$2,A2,$S$2,",",$S$2,B2,$S$2,",",TEXT(D2,"dd/mm/aaaa"),",",$S$2,E2,$S$2,",",$S$2,F2,$S$2,",",$S$2,G2,$S$2,",",$S$2,H2,$S$2,",",$S$2,I2,$S$2,",",$S$2,J2,$S$2)</f>
+        <v>INSERT INTO 'persona' VALUES ("Usmar Isacc","Miguel","Lopez",16/10/1999,"M","LopezMiguelUs@gmail.com","9718643085","direccion prueba","Ixtepec","/directory/img-person/UsmarIsaccMiguel.jpg"</v>
+      </c>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7">
+        <v>36261</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F26" si="0">CONCATENATE(B3,A3,LEFT(C3,2),"@gmail.com")</f>
+        <v>LopezMoralesGi@gmail.com</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G26" ca="1" si="1">CONCATENATE("971",RANDBETWEEN(1111111,9999999))</f>
+        <v>9716537884</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L26" ca="1" si="2">CONCATENATE("INSERT INTO 'persona' VALUES (",$S$2,C3,$S$2,",",$S$2,A3,$S$2,",",$S$2,B3,$S$2,",",TEXT(D3,"dd/mm/aaaa"),",",$S$2,E3,$S$2,",",$S$2,F3,$S$2,",",$S$2,G3,$S$2,",",$S$2,H3,$S$2,",",$S$2,I3,$S$2,",",$S$2,J3,$S$2)</f>
+        <v>INSERT INTO 'persona' VALUES ("Giovanni Alexander","Morales","Lopez",11/04/1999,"M","LopezMoralesGi@gmail.com","9716537884","direccion prueba","Ixtaltepec","/directory/img-person/GiovanniAlexanderMorales.jpg"</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7">
+        <v>35921</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>OrozcoMoralesRo@gmail.com</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9714398190</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" t="s">
+        <v>184</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Roel","Morales","Orozco",06/05/1998,"M","OrozcoMoralesRo@gmail.com","9714398190","direccion prueba","Juchitán","/directory/img-person/RoelMorales.jpg"</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7">
+        <v>36287</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>SilvaNuñezKa@gmail.com</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9717375329</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J5" t="s">
+        <v>185</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Karina","Nuñez","Silva",07/05/1999,"F","SilvaNuñezKa@gmail.com","9717375329","direccion prueba","Ixtepec","/directory/img-person/KarinaNuñez.jpg"</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7">
+        <v>36464</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>CruzOrozcoKe@gmail.com</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9719281395</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I6" t="s">
+        <v>181</v>
+      </c>
+      <c r="J6" t="s">
+        <v>186</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Kenia","Orozco","Cruz",31/10/1999,"F","CruzOrozcoKe@gmail.com","9719281395","direccion prueba","Salina Cruz","/directory/img-person/KeniaOrozco.jpg"</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7">
+        <v>36183</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>BautistaOrozcoDe@gmail.com</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9717008084</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I7" t="s">
+        <v>174</v>
+      </c>
+      <c r="J7" t="s">
+        <v>197</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Dennis Sabas","Orozco","Bautista",23/01/1999,"F","BautistaOrozcoDe@gmail.com","9717008084","direccion prueba","Juchitán","/directory/img-person/DennisSabasOrozco.jpg"</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="7">
+        <v>36297</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>MatusOrtizCa@gmail.com</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9712999067</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I8" t="s">
+        <v>181</v>
+      </c>
+      <c r="J8" t="s">
+        <v>198</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Carlos Roberto","Ortiz","Matus",17/05/1999,"M","MatusOrtizCa@gmail.com","9712999067","direccion prueba","Salina Cruz","/directory/img-person/CarlosRobertoOrtiz.jpg"</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="7">
+        <v>35918</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>SolanoAltamiranoIs@gmail.com</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9711943292</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I9" t="s">
+        <v>176</v>
+      </c>
+      <c r="J9" t="s">
+        <v>199</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Isis Yamile","Altamirano","Solano",03/05/1998,"F","SolanoAltamiranoIs@gmail.com","9711943292","direccion prueba","Ixtepec","/directory/img-person/IsisYamileAltamirano.jpg"</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="7">
+        <v>36168</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>SanchezAntinioFá@gmail.com</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9715837104</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J10" t="s">
+        <v>187</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Fátima","Antinio","Sanchez",08/01/1999,"F","SanchezAntinioFá@gmail.com","9715837104","direccion prueba","Juchitán","/directory/img-person/FátimaAntinio.jpg"</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="7">
+        <v>36521</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>CruzAquinoIt@gmail.com</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9714814547</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I11" t="s">
+        <v>179</v>
+      </c>
+      <c r="J11" t="s">
+        <v>200</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Itzury Alejandra","Aquino","Cruz",27/12/1999,"F","CruzAquinoIt@gmail.com","9714814547","direccion prueba","Chicapa","/directory/img-person/ItzuryAlejandraAquino.jpg"</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7">
+        <v>36444</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>RegaladoAquinoVi@gmail.com</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9712836224</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I12" t="s">
+        <v>174</v>
+      </c>
+      <c r="J12" t="s">
+        <v>188</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Vicente","Aquino","Regalado",11/10/1999,"M","RegaladoAquinoVi@gmail.com","9712836224","direccion prueba","Juchitán","/directory/img-person/VicenteAquino.jpg"</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="7">
+        <v>36497</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>BenitezAranjoBa@gmail.com</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9718294495</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I13" t="s">
+        <v>177</v>
+      </c>
+      <c r="J13" t="s">
+        <v>189</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Baudel","Aranjo","Benitez",03/12/1999,"M","BenitezAranjoBa@gmail.com","9718294495","direccion prueba","Espinal","/directory/img-person/BaudelAranjo.jpg"</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="7">
+        <v>36478</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>MoralesAvedañoYo@gmail.com</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9711830655</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I14" t="s">
+        <v>180</v>
+      </c>
+      <c r="J14" t="s">
+        <v>201</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Yosmar Manuel","Avedaño","Morales",14/11/1999,"M","MoralesAvedañoYo@gmail.com","9711830655","direccion prueba","Ixtaltepec","/directory/img-person/YosmarManuelAvedaño.jpg"</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="7">
+        <v>36367</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>MoralesBenefieldBr@gmail.com</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9718085542</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I15" t="s">
+        <v>178</v>
+      </c>
+      <c r="J15" t="s">
+        <v>190</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Brian","Benefield","Morales",26/07/1999,"M","MoralesBenefieldBr@gmail.com","9718085542","direccion prueba","Unión Hidalgo","/directory/img-person/BrianBenefield.jpg"</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="7">
+        <v>35984</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>VelasquezZarateKe@gmail.com</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9714804363</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I16" t="s">
+        <v>179</v>
+      </c>
+      <c r="J16" t="s">
+        <v>202</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Kevin Gabriel","Zarate","Velasquez",08/07/1998,"M","VelasquezZarateKe@gmail.com","9714804363","direccion prueba","Chicapa","/directory/img-person/KevinGabrielZarate.jpg"</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="7">
+        <v>36273</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>VillalobosZarateJe@gmail.com</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9716652321</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J17" t="s">
+        <v>203</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Jesus Antonio","Zarate","Villalobos",23/04/1999,"M","VillalobosZarateJe@gmail.com","9716652321","direccion prueba","Juchitán","/directory/img-person/JesusAntonioZarate.jpg"</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="7">
+        <v>36404</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>JiménezZavalaCl@gmail.com</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9713136729</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I18" t="s">
+        <v>179</v>
+      </c>
+      <c r="J18" t="s">
+        <v>191</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Clarissa","Zavala","Jiménez",01/09/1999,"F","JiménezZavalaCl@gmail.com","9713136729","direccion prueba","Chicapa","/directory/img-person/ClarissaZavala.jpg"</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="7">
+        <v>36314</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>UlisesAguilarAl@gmail.com</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9713795592</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I19" t="s">
+        <v>176</v>
+      </c>
+      <c r="J19" t="s">
+        <v>204</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Alba Beatriz","Aguilar","Ulises",03/06/1999,"F","UlisesAguilarAl@gmail.com","9713795592","direccion prueba","Ixtepec","/directory/img-person/AlbaBeatrizAguilar.jpg"</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="7">
+        <v>36515</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>de JesusFuentesLu@gmail.com</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9712832723</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I20" t="s">
+        <v>177</v>
+      </c>
+      <c r="J20" t="s">
+        <v>192</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Luis","Fuentes","de Jesus",21/12/1999,"M","de JesusFuentesLu@gmail.com","9712832723","direccion prueba","Espinal","/directory/img-person/LuisFuentes.jpg"</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="7">
+        <v>36491</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>RosadoRevueltaMa@gmail.com</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9715824747</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I21" t="s">
+        <v>174</v>
+      </c>
+      <c r="J21" t="s">
+        <v>193</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Maytor","Revuelta","Rosado",27/11/1999,"M","RosadoRevueltaMa@gmail.com","9715824747","direccion prueba","Juchitán","/directory/img-person/MaytorRevuelta.jpg"</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="7">
+        <v>36277</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>LuisRoblesJo@gmail.com</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9719591540</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I22" t="s">
+        <v>175</v>
+      </c>
+      <c r="J22" t="s">
+        <v>194</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Jorge","Robles","Luis",27/04/1999,"M","LuisRoblesJo@gmail.com","9719591540","direccion prueba","Tehuantepec","/directory/img-person/JorgeRobles.jpg"</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="7">
+        <v>36126</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>EscobarRodasSe@gmail.com</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9718285338</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I23" t="s">
+        <v>178</v>
+      </c>
+      <c r="J23" t="s">
+        <v>195</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Sergio","Rodas","Escobar",27/11/1998,"M","EscobarRodasSe@gmail.com","9718285338","direccion prueba","Unión Hidalgo","/directory/img-person/SergioRodas.jpg"</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="7">
+        <v>36168</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>SanchezRuizBr@gmail.com</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9711479144</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I24" t="s">
+        <v>180</v>
+      </c>
+      <c r="J24" t="s">
+        <v>205</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Brisa Donaji","Ruiz","Sanchez",08/01/1999,"F","SanchezRuizBr@gmail.com","9711479144","direccion prueba","Ixtaltepec","/directory/img-person/BrisaDonajiRuiz.jpg"</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="7">
+        <v>36445</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>VicenteRuizJa@gmail.com</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9717657524</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I25" t="s">
+        <v>175</v>
+      </c>
+      <c r="J25" t="s">
+        <v>206</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("Jair Michael","Ruiz","Vicente",12/10/1999,"M","VicenteRuizJa@gmail.com","9717657524","direccion prueba","Tehuantepec","/directory/img-person/JairMichaelRuiz.jpg"</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="7">
+        <v>36182</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>LopezGonzalesJo@gmail.com</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>9714045796</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I26" t="s">
+        <v>174</v>
+      </c>
+      <c r="J26" t="s">
+        <v>207</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>INSERT INTO 'persona' VALUES ("José Guillermo","Gonzales","Lopez",22/01/1999,"M","LopezGonzalesJo@gmail.com","9714045796","direccion prueba","Juchitán","/directory/img-person/JoséGuillermoGonzales.jpg"</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>